<commit_message>
add esercizio d6 e modifica QUARTO ESERCIZIO
</commit_message>
<xml_diff>
--- a/QUARTO ESERCIZIO.xlsx
+++ b/QUARTO ESERCIZIO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emanuele\OneDrive\Desktop\Epicode Exercise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F3E028-191E-4F40-8502-58B35E0150C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED961DA-DCB5-418D-A0E6-6D49BB4AD19C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assoluti_Iva" sheetId="15" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="242">
   <si>
     <t>mese</t>
   </si>
@@ -6769,8 +6769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6821,6 +6821,10 @@
       <c r="E2" s="27">
         <v>23</v>
       </c>
+      <c r="F2" s="25" t="str">
+        <f>IF(AND(A2="gennaio",C2="casa",E2&gt;10),"Trovato","")</f>
+        <v/>
+      </c>
       <c r="G2" s="42" t="s">
         <v>225</v>
       </c>
@@ -6846,8 +6850,9 @@
       <c r="E3" s="27">
         <v>25</v>
       </c>
-      <c r="F3" s="25" t="s">
-        <v>241</v>
+      <c r="F3" s="25" t="str">
+        <f t="shared" ref="F3:F24" si="0">IF(AND(A3="gennaio",C3="casa",E3&gt;10),"Trovato","")</f>
+        <v>Trovato</v>
       </c>
       <c r="G3" s="43"/>
       <c r="H3" s="43"/>
@@ -6872,6 +6877,10 @@
       <c r="E4" s="27">
         <v>69</v>
       </c>
+      <c r="F4" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="G4" s="43"/>
       <c r="H4" s="43"/>
       <c r="I4" s="43"/>
@@ -6895,6 +6904,10 @@
       <c r="E5" s="27">
         <v>554</v>
       </c>
+      <c r="F5" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="G5" s="43"/>
       <c r="H5" s="43"/>
       <c r="I5" s="43"/>
@@ -6918,8 +6931,9 @@
       <c r="E6" s="27">
         <v>569</v>
       </c>
-      <c r="F6" s="25" t="s">
-        <v>241</v>
+      <c r="F6" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>Trovato</v>
       </c>
       <c r="G6" s="43"/>
       <c r="H6" s="43"/>
@@ -6944,6 +6958,10 @@
       <c r="E7" s="27">
         <v>58</v>
       </c>
+      <c r="F7" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="G7" s="43"/>
       <c r="H7" s="43"/>
       <c r="I7" s="43"/>
@@ -6967,8 +6985,9 @@
       <c r="E8" s="27">
         <v>885</v>
       </c>
-      <c r="F8" s="25" t="s">
-        <v>241</v>
+      <c r="F8" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>Trovato</v>
       </c>
       <c r="G8" s="43"/>
       <c r="H8" s="43"/>
@@ -6993,6 +7012,10 @@
       <c r="E9" s="27">
         <v>821</v>
       </c>
+      <c r="F9" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
@@ -7010,6 +7033,10 @@
       <c r="E10" s="27">
         <v>23</v>
       </c>
+      <c r="F10" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
@@ -7027,6 +7054,10 @@
       <c r="E11" s="27">
         <v>36</v>
       </c>
+      <c r="F11" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
@@ -7044,6 +7075,10 @@
       <c r="E12" s="27">
         <v>5</v>
       </c>
+      <c r="F12" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="25" t="s">
@@ -7061,6 +7096,10 @@
       <c r="E13" s="27">
         <v>266</v>
       </c>
+      <c r="F13" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="25" t="s">
@@ -7078,6 +7117,10 @@
       <c r="E14" s="27">
         <v>221</v>
       </c>
+      <c r="F14" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="25" t="s">
@@ -7095,6 +7138,10 @@
       <c r="E15" s="27">
         <v>56</v>
       </c>
+      <c r="F15" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="25" t="s">
@@ -7112,8 +7159,12 @@
       <c r="E16" s="27">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="25" t="s">
         <v>19</v>
       </c>
@@ -7129,8 +7180,12 @@
       <c r="E17" s="27">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="25" t="s">
         <v>26</v>
       </c>
@@ -7146,8 +7201,12 @@
       <c r="E18" s="27">
         <v>72.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="25" t="s">
         <v>26</v>
       </c>
@@ -7163,8 +7222,12 @@
       <c r="E19" s="27">
         <v>30</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="25" t="s">
         <v>26</v>
       </c>
@@ -7180,8 +7243,12 @@
       <c r="E20" s="27">
         <v>51</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="25" t="s">
         <v>26</v>
       </c>
@@ -7197,8 +7264,12 @@
       <c r="E21" s="27">
         <v>14</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="25" t="s">
         <v>26</v>
       </c>
@@ -7214,8 +7285,12 @@
       <c r="E22" s="27">
         <v>75</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="25" t="s">
         <v>26</v>
       </c>
@@ -7231,8 +7306,12 @@
       <c r="E23" s="27">
         <v>270</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="25" t="s">
         <v>26</v>
       </c>
@@ -7247,6 +7326,10 @@
       </c>
       <c r="E24" s="27">
         <v>20</v>
+      </c>
+      <c r="F24" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -7262,7 +7345,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CBD8C3F-135D-4280-BD95-8C23E6C981DD}">
   <dimension ref="A1:E111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
modifiche esercizi 3 e 4
</commit_message>
<xml_diff>
--- a/QUARTO ESERCIZIO.xlsx
+++ b/QUARTO ESERCIZIO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emanuele\OneDrive\Desktop\Epicode Exercise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED961DA-DCB5-418D-A0E6-6D49BB4AD19C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9555CD-E3BE-43B7-BDFB-E14EC0D90D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="242">
   <si>
     <t>mese</t>
   </si>
@@ -1098,7 +1098,6 @@
     <xf numFmtId="173" fontId="2" fillId="0" borderId="0" xfId="6" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="6" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="171" fontId="2" fillId="2" borderId="0" xfId="10" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="6" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1115,6 +1114,7 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="171" fontId="2" fillId="6" borderId="0" xfId="10" applyFill="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Comma [0]" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1129,7 +1129,22 @@
     <cellStyle name="Valuta 2" xfId="7" xr:uid="{207091F5-721C-455F-B370-D6B4AD03B231}"/>
     <cellStyle name="Valuta_gestione clienti(out)-1" xfId="4" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1467,14 +1482,14 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
+      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="41.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="54.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" style="7" bestFit="1" customWidth="1"/>
@@ -1483,18 +1498,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="102.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="40" t="s">
         <v>214</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
       <c r="E3" s="7" t="s">
         <v>236</v>
       </c>
@@ -1538,7 +1553,7 @@
       <c r="B5" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="37">
+      <c r="C5" s="43">
         <v>281000</v>
       </c>
       <c r="D5" s="7" t="s">
@@ -1564,7 +1579,7 @@
       <c r="B6" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="37">
+      <c r="C6" s="43">
         <v>323000</v>
       </c>
       <c r="D6" s="7" t="s">
@@ -1590,7 +1605,7 @@
       <c r="B7" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="37">
+      <c r="C7" s="43">
         <v>344000</v>
       </c>
       <c r="D7" s="7" t="s">
@@ -1616,7 +1631,7 @@
       <c r="B8" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="37">
+      <c r="C8" s="43">
         <v>361000</v>
       </c>
     </row>
@@ -1627,7 +1642,7 @@
       <c r="B9" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="37">
+      <c r="C9" s="43">
         <v>521000</v>
       </c>
     </row>
@@ -1638,7 +1653,7 @@
       <c r="B10" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="37">
+      <c r="C10" s="43">
         <v>527000</v>
       </c>
     </row>
@@ -1649,7 +1664,7 @@
       <c r="B11" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="37">
+      <c r="C11" s="43">
         <v>626000</v>
       </c>
     </row>
@@ -1660,7 +1675,7 @@
       <c r="B12" t="s">
         <v>68</v>
       </c>
-      <c r="C12" s="37">
+      <c r="C12" s="43">
         <v>656000</v>
       </c>
     </row>
@@ -1671,7 +1686,7 @@
       <c r="B13" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="37">
+      <c r="C13" s="43">
         <v>666000</v>
       </c>
     </row>
@@ -1682,7 +1697,7 @@
       <c r="B14" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="37">
+      <c r="C14" s="43">
         <v>882000</v>
       </c>
     </row>
@@ -1693,7 +1708,7 @@
       <c r="B15" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="37">
+      <c r="C15" s="43">
         <v>1108000</v>
       </c>
     </row>
@@ -1704,7 +1719,7 @@
       <c r="B16" t="s">
         <v>78</v>
       </c>
-      <c r="C16" s="37">
+      <c r="C16" s="43">
         <v>1316000</v>
       </c>
     </row>
@@ -1715,7 +1730,7 @@
       <c r="B17" t="s">
         <v>98</v>
       </c>
-      <c r="C17" s="37">
+      <c r="C17" s="43">
         <v>1594000</v>
       </c>
     </row>
@@ -1726,7 +1741,7 @@
       <c r="B18" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="37">
+      <c r="C18" s="43">
         <v>2719000</v>
       </c>
     </row>
@@ -1737,7 +1752,7 @@
       <c r="B19" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="37">
+      <c r="C19" s="43">
         <v>0</v>
       </c>
     </row>
@@ -1748,7 +1763,7 @@
       <c r="B20" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="37">
+      <c r="C20" s="43">
         <v>4092000</v>
       </c>
     </row>
@@ -1759,7 +1774,7 @@
       <c r="B21" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="37">
+      <c r="C21" s="43">
         <v>13859000</v>
       </c>
     </row>
@@ -1770,7 +1785,7 @@
       <c r="B22" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="37">
+      <c r="C22" s="43">
         <v>0</v>
       </c>
     </row>
@@ -1781,7 +1796,7 @@
       <c r="B23" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="37">
+      <c r="C23" s="43">
         <v>167000</v>
       </c>
     </row>
@@ -1792,7 +1807,7 @@
       <c r="B24" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="37">
+      <c r="C24" s="43">
         <v>202000</v>
       </c>
     </row>
@@ -1803,7 +1818,7 @@
       <c r="B25" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="37">
+      <c r="C25" s="43">
         <v>203000</v>
       </c>
     </row>
@@ -1814,7 +1829,7 @@
       <c r="B26" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="37">
+      <c r="C26" s="43">
         <v>234000</v>
       </c>
     </row>
@@ -1825,7 +1840,7 @@
       <c r="B27" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="37">
+      <c r="C27" s="43">
         <v>252000</v>
       </c>
     </row>
@@ -1836,7 +1851,7 @@
       <c r="B28" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="37">
+      <c r="C28" s="43">
         <v>259000</v>
       </c>
     </row>
@@ -1847,7 +1862,7 @@
       <c r="B29" t="s">
         <v>68</v>
       </c>
-      <c r="C29" s="37">
+      <c r="C29" s="43">
         <v>269000</v>
       </c>
     </row>
@@ -1858,7 +1873,7 @@
       <c r="B30" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="37">
+      <c r="C30" s="43">
         <v>271000</v>
       </c>
     </row>
@@ -1869,7 +1884,7 @@
       <c r="B31" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="37">
+      <c r="C31" s="43">
         <v>292000</v>
       </c>
     </row>
@@ -1880,7 +1895,7 @@
       <c r="B32" t="s">
         <v>36</v>
       </c>
-      <c r="C32" s="37">
+      <c r="C32" s="43">
         <v>293000</v>
       </c>
     </row>
@@ -1891,7 +1906,7 @@
       <c r="B33" t="s">
         <v>78</v>
       </c>
-      <c r="C33" s="37">
+      <c r="C33" s="43">
         <v>307000</v>
       </c>
     </row>
@@ -1902,7 +1917,7 @@
       <c r="B34" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="37">
+      <c r="C34" s="43">
         <v>440000</v>
       </c>
     </row>
@@ -1913,7 +1928,7 @@
       <c r="B35" t="s">
         <v>60</v>
       </c>
-      <c r="C35" s="37">
+      <c r="C35" s="43">
         <v>487000</v>
       </c>
     </row>
@@ -1924,7 +1939,7 @@
       <c r="B36" t="s">
         <v>60</v>
       </c>
-      <c r="C36" s="37">
+      <c r="C36" s="43">
         <v>566000</v>
       </c>
     </row>
@@ -1935,7 +1950,7 @@
       <c r="B37" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="37">
+      <c r="C37" s="43">
         <v>802000</v>
       </c>
     </row>
@@ -1946,7 +1961,7 @@
       <c r="B38" t="s">
         <v>49</v>
       </c>
-      <c r="C38" s="37">
+      <c r="C38" s="43">
         <v>1579000</v>
       </c>
     </row>
@@ -1957,7 +1972,7 @@
       <c r="B39" t="s">
         <v>60</v>
       </c>
-      <c r="C39" s="37">
+      <c r="C39" s="43">
         <v>0</v>
       </c>
     </row>
@@ -1968,7 +1983,7 @@
       <c r="B40" t="s">
         <v>98</v>
       </c>
-      <c r="C40" s="37">
+      <c r="C40" s="43">
         <v>70000</v>
       </c>
     </row>
@@ -1979,7 +1994,7 @@
       <c r="B41" t="s">
         <v>52</v>
       </c>
-      <c r="C41" s="37">
+      <c r="C41" s="43">
         <v>104000</v>
       </c>
     </row>
@@ -1990,7 +2005,7 @@
       <c r="B42" t="s">
         <v>54</v>
       </c>
-      <c r="C42" s="37">
+      <c r="C42" s="43">
         <v>127000</v>
       </c>
     </row>
@@ -2001,7 +2016,7 @@
       <c r="B43" t="s">
         <v>73</v>
       </c>
-      <c r="C43" s="37">
+      <c r="C43" s="43">
         <v>162000</v>
       </c>
     </row>
@@ -2012,7 +2027,7 @@
       <c r="B44" t="s">
         <v>68</v>
       </c>
-      <c r="C44" s="37">
+      <c r="C44" s="43">
         <v>179000</v>
       </c>
     </row>
@@ -2023,7 +2038,7 @@
       <c r="B45" t="s">
         <v>88</v>
       </c>
-      <c r="C45" s="37">
+      <c r="C45" s="43">
         <v>186000</v>
       </c>
     </row>
@@ -2034,7 +2049,7 @@
       <c r="B46" t="s">
         <v>36</v>
       </c>
-      <c r="C46" s="37">
+      <c r="C46" s="43">
         <v>186000</v>
       </c>
     </row>
@@ -2045,7 +2060,7 @@
       <c r="B47" t="s">
         <v>40</v>
       </c>
-      <c r="C47" s="37">
+      <c r="C47" s="43">
         <v>203000</v>
       </c>
     </row>
@@ -2056,7 +2071,7 @@
       <c r="B48" t="s">
         <v>40</v>
       </c>
-      <c r="C48" s="37">
+      <c r="C48" s="43">
         <v>212000</v>
       </c>
     </row>
@@ -2067,7 +2082,7 @@
       <c r="B49" t="s">
         <v>81</v>
       </c>
-      <c r="C49" s="37">
+      <c r="C49" s="43">
         <v>222000</v>
       </c>
     </row>
@@ -2078,7 +2093,7 @@
       <c r="B50" t="s">
         <v>52</v>
       </c>
-      <c r="C50" s="37">
+      <c r="C50" s="43">
         <v>245000</v>
       </c>
     </row>
@@ -2089,7 +2104,7 @@
       <c r="B51" t="s">
         <v>68</v>
       </c>
-      <c r="C51" s="37">
+      <c r="C51" s="43">
         <v>251000</v>
       </c>
     </row>
@@ -2100,7 +2115,7 @@
       <c r="B52" t="s">
         <v>81</v>
       </c>
-      <c r="C52" s="37">
+      <c r="C52" s="43">
         <v>257000</v>
       </c>
     </row>
@@ -2111,7 +2126,7 @@
       <c r="B53" t="s">
         <v>81</v>
       </c>
-      <c r="C53" s="37">
+      <c r="C53" s="43">
         <v>269000</v>
       </c>
     </row>
@@ -2122,7 +2137,7 @@
       <c r="B54" t="s">
         <v>88</v>
       </c>
-      <c r="C54" s="37">
+      <c r="C54" s="43">
         <v>314000</v>
       </c>
     </row>
@@ -2130,10 +2145,10 @@
       <c r="A55" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B55" s="38" t="s">
+      <c r="B55" s="37" t="s">
         <v>240</v>
       </c>
-      <c r="C55" s="37">
+      <c r="C55" s="43">
         <v>325000</v>
       </c>
     </row>
@@ -2144,7 +2159,7 @@
       <c r="B56" t="s">
         <v>36</v>
       </c>
-      <c r="C56" s="37">
+      <c r="C56" s="43">
         <v>347000</v>
       </c>
     </row>
@@ -2155,7 +2170,7 @@
       <c r="B57" t="s">
         <v>36</v>
       </c>
-      <c r="C57" s="37">
+      <c r="C57" s="43">
         <v>369000</v>
       </c>
     </row>
@@ -2166,7 +2181,7 @@
       <c r="B58" t="s">
         <v>36</v>
       </c>
-      <c r="C58" s="37">
+      <c r="C58" s="43">
         <v>402000</v>
       </c>
     </row>
@@ -2177,7 +2192,7 @@
       <c r="B59" t="s">
         <v>78</v>
       </c>
-      <c r="C59" s="37">
+      <c r="C59" s="43">
         <v>471000</v>
       </c>
     </row>
@@ -2188,7 +2203,7 @@
       <c r="B60" t="s">
         <v>56</v>
       </c>
-      <c r="C60" s="37">
+      <c r="C60" s="43">
         <v>476000</v>
       </c>
     </row>
@@ -2199,7 +2214,7 @@
       <c r="B61" t="s">
         <v>94</v>
       </c>
-      <c r="C61" s="37">
+      <c r="C61" s="43">
         <v>492000</v>
       </c>
     </row>
@@ -2210,7 +2225,7 @@
       <c r="B62" t="s">
         <v>81</v>
       </c>
-      <c r="C62" s="37">
+      <c r="C62" s="43">
         <v>531000</v>
       </c>
     </row>
@@ -2221,7 +2236,7 @@
       <c r="B63" t="s">
         <v>36</v>
       </c>
-      <c r="C63" s="37">
+      <c r="C63" s="43">
         <v>552000</v>
       </c>
     </row>
@@ -2232,7 +2247,7 @@
       <c r="B64" t="s">
         <v>40</v>
       </c>
-      <c r="C64" s="37">
+      <c r="C64" s="43">
         <v>1487000</v>
       </c>
     </row>
@@ -2243,7 +2258,7 @@
       <c r="B65" t="s">
         <v>94</v>
       </c>
-      <c r="C65" s="37">
+      <c r="C65" s="43">
         <v>0</v>
       </c>
     </row>
@@ -2254,7 +2269,7 @@
       <c r="B66" t="s">
         <v>40</v>
       </c>
-      <c r="C66" s="37">
+      <c r="C66" s="43">
         <v>101000</v>
       </c>
     </row>
@@ -2265,7 +2280,7 @@
       <c r="B67" t="s">
         <v>88</v>
       </c>
-      <c r="C67" s="37">
+      <c r="C67" s="43">
         <v>38000</v>
       </c>
     </row>
@@ -2276,7 +2291,7 @@
       <c r="B68" t="s">
         <v>88</v>
       </c>
-      <c r="C68" s="37">
+      <c r="C68" s="43">
         <v>137000</v>
       </c>
     </row>
@@ -2287,7 +2302,7 @@
       <c r="B69" t="s">
         <v>94</v>
       </c>
-      <c r="C69" s="37">
+      <c r="C69" s="43">
         <v>222000</v>
       </c>
     </row>
@@ -2298,7 +2313,7 @@
       <c r="B70" t="s">
         <v>102</v>
       </c>
-      <c r="C70" s="37">
+      <c r="C70" s="43">
         <v>501000</v>
       </c>
     </row>
@@ -2309,7 +2324,7 @@
       <c r="B71" t="s">
         <v>58</v>
       </c>
-      <c r="C71" s="37">
+      <c r="C71" s="43">
         <v>428000</v>
       </c>
     </row>
@@ -2320,7 +2335,7 @@
       <c r="B72" t="s">
         <v>68</v>
       </c>
-      <c r="C72" s="37">
+      <c r="C72" s="43">
         <v>561000</v>
       </c>
     </row>
@@ -2331,7 +2346,7 @@
       <c r="B73" t="s">
         <v>68</v>
       </c>
-      <c r="C73" s="37">
+      <c r="C73" s="43">
         <v>1578000</v>
       </c>
     </row>
@@ -2342,7 +2357,7 @@
       <c r="B74" t="s">
         <v>54</v>
       </c>
-      <c r="C74" s="37">
+      <c r="C74" s="43">
         <v>34000</v>
       </c>
     </row>
@@ -2353,7 +2368,7 @@
       <c r="B75" t="s">
         <v>102</v>
       </c>
-      <c r="C75" s="37">
+      <c r="C75" s="43">
         <v>20000</v>
       </c>
     </row>
@@ -2364,7 +2379,7 @@
       <c r="B76" t="s">
         <v>56</v>
       </c>
-      <c r="C76" s="37">
+      <c r="C76" s="43">
         <v>23000</v>
       </c>
     </row>
@@ -2375,7 +2390,7 @@
       <c r="B77" t="s">
         <v>94</v>
       </c>
-      <c r="C77" s="37">
+      <c r="C77" s="43">
         <v>98000</v>
       </c>
     </row>
@@ -2386,7 +2401,7 @@
       <c r="B78" t="s">
         <v>58</v>
       </c>
-      <c r="C78" s="37">
+      <c r="C78" s="43">
         <v>251000</v>
       </c>
     </row>
@@ -2397,7 +2412,7 @@
       <c r="B79" t="s">
         <v>36</v>
       </c>
-      <c r="C79" s="37">
+      <c r="C79" s="43">
         <v>15000</v>
       </c>
     </row>
@@ -2408,7 +2423,7 @@
       <c r="B80" t="s">
         <v>52</v>
       </c>
-      <c r="C80" s="37">
+      <c r="C80" s="43">
         <v>14000</v>
       </c>
     </row>
@@ -2419,7 +2434,7 @@
       <c r="B81" t="s">
         <v>68</v>
       </c>
-      <c r="C81" s="37">
+      <c r="C81" s="43">
         <v>0</v>
       </c>
     </row>
@@ -2430,7 +2445,7 @@
       <c r="B82" t="s">
         <v>68</v>
       </c>
-      <c r="C82" s="37">
+      <c r="C82" s="43">
         <v>399000</v>
       </c>
     </row>
@@ -2441,7 +2456,7 @@
       <c r="B83" t="s">
         <v>94</v>
       </c>
-      <c r="C83" s="37">
+      <c r="C83" s="43">
         <v>259000</v>
       </c>
     </row>
@@ -2452,7 +2467,7 @@
       <c r="B84" t="s">
         <v>36</v>
       </c>
-      <c r="C84" s="37">
+      <c r="C84" s="43">
         <v>324000</v>
       </c>
     </row>
@@ -2463,7 +2478,7 @@
       <c r="B85" t="s">
         <v>36</v>
       </c>
-      <c r="C85" s="37">
+      <c r="C85" s="43">
         <v>378000</v>
       </c>
     </row>
@@ -2474,7 +2489,7 @@
       <c r="B86" t="s">
         <v>68</v>
       </c>
-      <c r="C86" s="37">
+      <c r="C86" s="43">
         <v>469000</v>
       </c>
     </row>
@@ -2485,7 +2500,7 @@
       <c r="B87" t="s">
         <v>58</v>
       </c>
-      <c r="C87" s="37">
+      <c r="C87" s="43">
         <v>556000</v>
       </c>
     </row>
@@ -2496,7 +2511,7 @@
       <c r="B88" t="s">
         <v>56</v>
       </c>
-      <c r="C88" s="37">
+      <c r="C88" s="43">
         <v>476000</v>
       </c>
     </row>
@@ -2507,7 +2522,7 @@
       <c r="B89" t="s">
         <v>44</v>
       </c>
-      <c r="C89" s="37">
+      <c r="C89" s="43">
         <v>477000</v>
       </c>
     </row>
@@ -2518,7 +2533,7 @@
       <c r="B90" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="C90" s="37">
+      <c r="C90" s="43">
         <v>556000</v>
       </c>
     </row>
@@ -2529,7 +2544,7 @@
       <c r="B91" t="s">
         <v>68</v>
       </c>
-      <c r="C91" s="37">
+      <c r="C91" s="43">
         <v>695000</v>
       </c>
     </row>
@@ -2540,7 +2555,7 @@
       <c r="B92" t="s">
         <v>46</v>
       </c>
-      <c r="C92" s="37">
+      <c r="C92" s="43">
         <v>1279000</v>
       </c>
     </row>
@@ -2551,7 +2566,7 @@
       <c r="B93" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="C93" s="37">
+      <c r="C93" s="43">
         <v>35000</v>
       </c>
     </row>
@@ -2562,7 +2577,7 @@
       <c r="B94" t="s">
         <v>38</v>
       </c>
-      <c r="C94" s="37">
+      <c r="C94" s="43">
         <v>175000</v>
       </c>
     </row>
@@ -2573,7 +2588,7 @@
       <c r="B95" t="s">
         <v>78</v>
       </c>
-      <c r="C95" s="37">
+      <c r="C95" s="43">
         <v>272000</v>
       </c>
     </row>
@@ -2584,7 +2599,7 @@
       <c r="B96" t="s">
         <v>98</v>
       </c>
-      <c r="C96" s="37">
+      <c r="C96" s="43">
         <v>198000</v>
       </c>
     </row>
@@ -2595,7 +2610,7 @@
       <c r="B97" t="s">
         <v>68</v>
       </c>
-      <c r="C97" s="37">
+      <c r="C97" s="43">
         <v>290000</v>
       </c>
     </row>
@@ -2606,7 +2621,7 @@
       <c r="B98" t="s">
         <v>42</v>
       </c>
-      <c r="C98" s="37">
+      <c r="C98" s="43">
         <v>589000</v>
       </c>
     </row>
@@ -2617,7 +2632,7 @@
       <c r="B99" t="s">
         <v>42</v>
       </c>
-      <c r="C99" s="37">
+      <c r="C99" s="43">
         <v>743000</v>
       </c>
     </row>
@@ -2628,7 +2643,7 @@
       <c r="B100" t="s">
         <v>52</v>
       </c>
-      <c r="C100" s="37">
+      <c r="C100" s="43">
         <v>271000</v>
       </c>
     </row>
@@ -2639,7 +2654,7 @@
       <c r="B101" t="s">
         <v>36</v>
       </c>
-      <c r="C101" s="37">
+      <c r="C101" s="43">
         <v>632000</v>
       </c>
     </row>
@@ -2650,7 +2665,7 @@
       <c r="B102" t="s">
         <v>56</v>
       </c>
-      <c r="C102" s="37">
+      <c r="C102" s="43">
         <v>90000</v>
       </c>
     </row>
@@ -2661,7 +2676,7 @@
       <c r="B103" t="s">
         <v>40</v>
       </c>
-      <c r="C103" s="37">
+      <c r="C103" s="43">
         <v>4000</v>
       </c>
     </row>
@@ -2672,7 +2687,7 @@
       <c r="B104" t="s">
         <v>68</v>
       </c>
-      <c r="C104" s="37">
+      <c r="C104" s="43">
         <v>5000</v>
       </c>
     </row>
@@ -2683,7 +2698,7 @@
       <c r="B105" t="s">
         <v>60</v>
       </c>
-      <c r="C105" s="37">
+      <c r="C105" s="43">
         <v>41000</v>
       </c>
     </row>
@@ -2694,7 +2709,7 @@
       <c r="B106" t="s">
         <v>60</v>
       </c>
-      <c r="C106" s="37">
+      <c r="C106" s="43">
         <v>0</v>
       </c>
     </row>
@@ -2705,7 +2720,7 @@
       <c r="B107" t="s">
         <v>36</v>
       </c>
-      <c r="C107" s="37">
+      <c r="C107" s="43">
         <v>737000</v>
       </c>
     </row>
@@ -2716,7 +2731,7 @@
       <c r="B108" t="s">
         <v>68</v>
       </c>
-      <c r="C108" s="37">
+      <c r="C108" s="43">
         <v>910000</v>
       </c>
     </row>
@@ -2727,7 +2742,7 @@
       <c r="B109" t="s">
         <v>60</v>
       </c>
-      <c r="C109" s="37">
+      <c r="C109" s="43">
         <v>241000</v>
       </c>
     </row>
@@ -2738,7 +2753,7 @@
       <c r="B110" t="s">
         <v>60</v>
       </c>
-      <c r="C110" s="37">
+      <c r="C110" s="43">
         <v>0</v>
       </c>
     </row>
@@ -2749,7 +2764,7 @@
       <c r="B111" t="s">
         <v>36</v>
       </c>
-      <c r="C111" s="37">
+      <c r="C111" s="43">
         <v>112000</v>
       </c>
     </row>
@@ -2760,7 +2775,7 @@
       <c r="B112" t="s">
         <v>78</v>
       </c>
-      <c r="C112" s="37">
+      <c r="C112" s="43">
         <v>113000</v>
       </c>
     </row>
@@ -2771,7 +2786,7 @@
       <c r="B113" t="s">
         <v>70</v>
       </c>
-      <c r="C113" s="37">
+      <c r="C113" s="43">
         <v>121000</v>
       </c>
     </row>
@@ -2782,7 +2797,7 @@
       <c r="B114" t="s">
         <v>60</v>
       </c>
-      <c r="C114" s="37">
+      <c r="C114" s="43">
         <v>160000</v>
       </c>
     </row>
@@ -2793,7 +2808,7 @@
       <c r="B115" t="s">
         <v>60</v>
       </c>
-      <c r="C115" s="37">
+      <c r="C115" s="43">
         <v>195000</v>
       </c>
     </row>
@@ -2804,7 +2819,7 @@
       <c r="B116" t="s">
         <v>40</v>
       </c>
-      <c r="C116" s="37">
+      <c r="C116" s="43">
         <v>215000</v>
       </c>
     </row>
@@ -2815,7 +2830,7 @@
       <c r="B117" t="s">
         <v>49</v>
       </c>
-      <c r="C117" s="37">
+      <c r="C117" s="43">
         <v>321000</v>
       </c>
     </row>
@@ -2826,7 +2841,7 @@
       <c r="B118" t="s">
         <v>60</v>
       </c>
-      <c r="C118" s="37">
+      <c r="C118" s="43">
         <v>614000</v>
       </c>
     </row>
@@ -2837,7 +2852,7 @@
       <c r="B119" t="s">
         <v>98</v>
       </c>
-      <c r="C119" s="37">
+      <c r="C119" s="43">
         <v>0</v>
       </c>
     </row>
@@ -2848,7 +2863,7 @@
       <c r="B120" t="s">
         <v>52</v>
       </c>
-      <c r="C120" s="37">
+      <c r="C120" s="43">
         <v>30000</v>
       </c>
     </row>
@@ -2859,7 +2874,7 @@
       <c r="B121" t="s">
         <v>54</v>
       </c>
-      <c r="C121" s="37">
+      <c r="C121" s="43">
         <v>34000</v>
       </c>
     </row>
@@ -2870,7 +2885,7 @@
       <c r="B122" t="s">
         <v>73</v>
       </c>
-      <c r="C122" s="37">
+      <c r="C122" s="43">
         <v>35000</v>
       </c>
     </row>
@@ -2881,7 +2896,7 @@
       <c r="B123" t="s">
         <v>68</v>
       </c>
-      <c r="C123" s="37">
+      <c r="C123" s="43">
         <v>77000</v>
       </c>
     </row>
@@ -2892,7 +2907,7 @@
       <c r="B124" t="s">
         <v>88</v>
       </c>
-      <c r="C124" s="37">
+      <c r="C124" s="43">
         <v>723000</v>
       </c>
     </row>
@@ -2903,7 +2918,7 @@
       <c r="B125" t="s">
         <v>36</v>
       </c>
-      <c r="C125" s="37">
+      <c r="C125" s="43">
         <v>742000</v>
       </c>
     </row>
@@ -2914,7 +2929,7 @@
       <c r="B126" t="s">
         <v>40</v>
       </c>
-      <c r="C126" s="37">
+      <c r="C126" s="43">
         <v>778000</v>
       </c>
     </row>
@@ -2925,7 +2940,7 @@
       <c r="B127" t="s">
         <v>40</v>
       </c>
-      <c r="C127" s="37">
+      <c r="C127" s="43">
         <v>878000</v>
       </c>
     </row>
@@ -2936,7 +2951,7 @@
       <c r="B128" t="s">
         <v>81</v>
       </c>
-      <c r="C128" s="37">
+      <c r="C128" s="43">
         <v>883000</v>
       </c>
     </row>
@@ -2947,7 +2962,7 @@
       <c r="B129" t="s">
         <v>52</v>
       </c>
-      <c r="C129" s="37">
+      <c r="C129" s="43">
         <v>913000</v>
       </c>
     </row>
@@ -2958,7 +2973,7 @@
       <c r="B130" t="s">
         <v>68</v>
       </c>
-      <c r="C130" s="37">
+      <c r="C130" s="43">
         <v>1125000</v>
       </c>
     </row>
@@ -2969,7 +2984,7 @@
       <c r="B131" t="s">
         <v>81</v>
       </c>
-      <c r="C131" s="37">
+      <c r="C131" s="43">
         <v>0</v>
       </c>
     </row>
@@ -2980,7 +2995,7 @@
       <c r="B132" t="s">
         <v>81</v>
       </c>
-      <c r="C132" s="37">
+      <c r="C132" s="43">
         <v>33000</v>
       </c>
     </row>
@@ -2991,7 +3006,7 @@
       <c r="B133" t="s">
         <v>88</v>
       </c>
-      <c r="C133" s="37">
+      <c r="C133" s="43">
         <v>52000</v>
       </c>
     </row>
@@ -2999,10 +3014,10 @@
       <c r="A134" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B134" s="38" t="s">
+      <c r="B134" s="37" t="s">
         <v>240</v>
       </c>
-      <c r="C134" s="37">
+      <c r="C134" s="43">
         <v>97000</v>
       </c>
     </row>
@@ -3013,7 +3028,7 @@
       <c r="B135" t="s">
         <v>36</v>
       </c>
-      <c r="C135" s="37">
+      <c r="C135" s="43">
         <v>0</v>
       </c>
     </row>
@@ -3024,7 +3039,7 @@
       <c r="B136" t="s">
         <v>36</v>
       </c>
-      <c r="C136" s="37">
+      <c r="C136" s="43">
         <v>131000</v>
       </c>
     </row>
@@ -3035,7 +3050,7 @@
       <c r="B137" t="s">
         <v>36</v>
       </c>
-      <c r="C137" s="37">
+      <c r="C137" s="43">
         <v>169000</v>
       </c>
     </row>
@@ -3046,7 +3061,7 @@
       <c r="B138" t="s">
         <v>78</v>
       </c>
-      <c r="C138" s="37">
+      <c r="C138" s="43">
         <v>190000</v>
       </c>
     </row>
@@ -3057,7 +3072,7 @@
       <c r="B139" t="s">
         <v>56</v>
       </c>
-      <c r="C139" s="37">
+      <c r="C139" s="43">
         <v>191000</v>
       </c>
     </row>
@@ -3068,7 +3083,7 @@
       <c r="B140" t="s">
         <v>94</v>
       </c>
-      <c r="C140" s="37">
+      <c r="C140" s="43">
         <v>197000</v>
       </c>
     </row>
@@ -3079,7 +3094,7 @@
       <c r="B141" t="s">
         <v>81</v>
       </c>
-      <c r="C141" s="37">
+      <c r="C141" s="43">
         <v>201000</v>
       </c>
     </row>
@@ -3090,7 +3105,7 @@
       <c r="B142" t="s">
         <v>36</v>
       </c>
-      <c r="C142" s="37">
+      <c r="C142" s="43">
         <v>220000</v>
       </c>
     </row>
@@ -3101,7 +3116,7 @@
       <c r="B143" t="s">
         <v>40</v>
       </c>
-      <c r="C143" s="37">
+      <c r="C143" s="43">
         <v>250000</v>
       </c>
     </row>
@@ -3112,7 +3127,7 @@
       <c r="B144" t="s">
         <v>94</v>
       </c>
-      <c r="C144" s="37">
+      <c r="C144" s="43">
         <v>257000</v>
       </c>
     </row>
@@ -3123,7 +3138,7 @@
       <c r="B145" t="s">
         <v>40</v>
       </c>
-      <c r="C145" s="37">
+      <c r="C145" s="43">
         <v>278000</v>
       </c>
     </row>
@@ -3134,7 +3149,7 @@
       <c r="B146" t="s">
         <v>88</v>
       </c>
-      <c r="C146" s="37">
+      <c r="C146" s="43">
         <v>280000</v>
       </c>
     </row>
@@ -3145,7 +3160,7 @@
       <c r="B147" t="s">
         <v>88</v>
       </c>
-      <c r="C147" s="37">
+      <c r="C147" s="43">
         <v>300000</v>
       </c>
     </row>
@@ -3156,7 +3171,7 @@
       <c r="B148" t="s">
         <v>94</v>
       </c>
-      <c r="C148" s="37">
+      <c r="C148" s="43">
         <v>305000</v>
       </c>
     </row>
@@ -3167,7 +3182,7 @@
       <c r="B149" t="s">
         <v>102</v>
       </c>
-      <c r="C149" s="37">
+      <c r="C149" s="43">
         <v>335000</v>
       </c>
     </row>
@@ -3178,7 +3193,7 @@
       <c r="B150" t="s">
         <v>58</v>
       </c>
-      <c r="C150" s="37">
+      <c r="C150" s="43">
         <v>360000</v>
       </c>
     </row>
@@ -3189,7 +3204,7 @@
       <c r="B151" t="s">
         <v>68</v>
       </c>
-      <c r="C151" s="37">
+      <c r="C151" s="43">
         <v>429000</v>
       </c>
     </row>
@@ -3200,7 +3215,7 @@
       <c r="B152" t="s">
         <v>68</v>
       </c>
-      <c r="C152" s="37">
+      <c r="C152" s="43">
         <v>701000</v>
       </c>
     </row>
@@ -3211,7 +3226,7 @@
       <c r="B153" t="s">
         <v>54</v>
       </c>
-      <c r="C153" s="37">
+      <c r="C153" s="43">
         <v>0</v>
       </c>
     </row>
@@ -3222,7 +3237,7 @@
       <c r="B154" t="s">
         <v>102</v>
       </c>
-      <c r="C154" s="37">
+      <c r="C154" s="43">
         <v>90000</v>
       </c>
     </row>
@@ -3233,7 +3248,7 @@
       <c r="B155" t="s">
         <v>56</v>
       </c>
-      <c r="C155" s="37">
+      <c r="C155" s="43">
         <v>69000</v>
       </c>
     </row>
@@ -3244,7 +3259,7 @@
       <c r="B156" t="s">
         <v>94</v>
       </c>
-      <c r="C156" s="37">
+      <c r="C156" s="43">
         <v>89000</v>
       </c>
     </row>
@@ -3255,7 +3270,7 @@
       <c r="B157" t="s">
         <v>58</v>
       </c>
-      <c r="C157" s="37">
+      <c r="C157" s="43">
         <v>138000</v>
       </c>
     </row>
@@ -3266,7 +3281,7 @@
       <c r="B158" t="s">
         <v>36</v>
       </c>
-      <c r="C158" s="37">
+      <c r="C158" s="43">
         <v>196000</v>
       </c>
     </row>
@@ -3277,7 +3292,7 @@
       <c r="B159" t="s">
         <v>52</v>
       </c>
-      <c r="C159" s="37">
+      <c r="C159" s="43">
         <v>329000</v>
       </c>
     </row>
@@ -3288,7 +3303,7 @@
       <c r="B160" t="s">
         <v>68</v>
       </c>
-      <c r="C160" s="37">
+      <c r="C160" s="43">
         <v>295000</v>
       </c>
     </row>
@@ -3299,7 +3314,7 @@
       <c r="B161" t="s">
         <v>68</v>
       </c>
-      <c r="C161" s="37">
+      <c r="C161" s="43">
         <v>19000</v>
       </c>
     </row>
@@ -3310,7 +3325,7 @@
       <c r="B162" t="s">
         <v>94</v>
       </c>
-      <c r="C162" s="37">
+      <c r="C162" s="43">
         <v>26000</v>
       </c>
     </row>
@@ -3321,7 +3336,7 @@
       <c r="B163" t="s">
         <v>36</v>
       </c>
-      <c r="C163" s="37">
+      <c r="C163" s="43">
         <v>28000</v>
       </c>
     </row>
@@ -3332,7 +3347,7 @@
       <c r="B164" t="s">
         <v>36</v>
       </c>
-      <c r="C164" s="37">
+      <c r="C164" s="43">
         <v>56000</v>
       </c>
     </row>
@@ -3343,7 +3358,7 @@
       <c r="B165" t="s">
         <v>68</v>
       </c>
-      <c r="C165" s="37">
+      <c r="C165" s="43">
         <v>0</v>
       </c>
     </row>
@@ -3354,7 +3369,7 @@
       <c r="B166" t="s">
         <v>58</v>
       </c>
-      <c r="C166" s="37">
+      <c r="C166" s="43">
         <v>216000</v>
       </c>
     </row>
@@ -3365,7 +3380,7 @@
       <c r="B167" t="s">
         <v>56</v>
       </c>
-      <c r="C167" s="37">
+      <c r="C167" s="43">
         <v>250000</v>
       </c>
     </row>
@@ -3376,7 +3391,7 @@
       <c r="B168" t="s">
         <v>44</v>
       </c>
-      <c r="C168" s="37">
+      <c r="C168" s="43">
         <v>382000</v>
       </c>
     </row>
@@ -3387,7 +3402,7 @@
       <c r="B169" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="C169" s="37">
+      <c r="C169" s="43">
         <v>524000</v>
       </c>
     </row>
@@ -3398,7 +3413,7 @@
       <c r="B170" t="s">
         <v>68</v>
       </c>
-      <c r="C170" s="37">
+      <c r="C170" s="43">
         <v>757000</v>
       </c>
     </row>
@@ -3409,7 +3424,7 @@
       <c r="B171" t="s">
         <v>46</v>
       </c>
-      <c r="C171" s="37">
+      <c r="C171" s="43">
         <v>1045000</v>
       </c>
     </row>
@@ -3420,7 +3435,7 @@
       <c r="B172" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="C172" s="37">
+      <c r="C172" s="43">
         <v>1568000</v>
       </c>
     </row>
@@ -3431,7 +3446,7 @@
       <c r="B173" t="s">
         <v>38</v>
       </c>
-      <c r="C173" s="37">
+      <c r="C173" s="43">
         <v>117000</v>
       </c>
     </row>
@@ -3442,7 +3457,7 @@
       <c r="B174" t="s">
         <v>78</v>
       </c>
-      <c r="C174" s="37">
+      <c r="C174" s="43">
         <v>158000</v>
       </c>
     </row>
@@ -3453,7 +3468,7 @@
       <c r="B175" t="s">
         <v>98</v>
       </c>
-      <c r="C175" s="37">
+      <c r="C175" s="43">
         <v>260000</v>
       </c>
     </row>
@@ -3464,7 +3479,7 @@
       <c r="B176" t="s">
         <v>68</v>
       </c>
-      <c r="C176" s="37">
+      <c r="C176" s="43">
         <v>193000</v>
       </c>
     </row>
@@ -3475,7 +3490,7 @@
       <c r="B177" t="s">
         <v>42</v>
       </c>
-      <c r="C177" s="37">
+      <c r="C177" s="43">
         <v>270000</v>
       </c>
     </row>
@@ -3486,7 +3501,7 @@
       <c r="B178" t="s">
         <v>42</v>
       </c>
-      <c r="C178" s="37">
+      <c r="C178" s="43">
         <v>314000</v>
       </c>
     </row>
@@ -3497,7 +3512,7 @@
       <c r="B179" t="s">
         <v>52</v>
       </c>
-      <c r="C179" s="37">
+      <c r="C179" s="43">
         <v>894000</v>
       </c>
     </row>
@@ -3508,7 +3523,7 @@
       <c r="B180" t="s">
         <v>36</v>
       </c>
-      <c r="C180" s="37">
+      <c r="C180" s="43">
         <v>1040000</v>
       </c>
     </row>
@@ -3519,7 +3534,7 @@
       <c r="B181" t="s">
         <v>56</v>
       </c>
-      <c r="C181" s="37">
+      <c r="C181" s="43">
         <v>8000</v>
       </c>
     </row>
@@ -3530,7 +3545,7 @@
       <c r="B182" t="s">
         <v>40</v>
       </c>
-      <c r="C182" s="37">
+      <c r="C182" s="43">
         <v>10000</v>
       </c>
     </row>
@@ -3541,7 +3556,7 @@
       <c r="B183" t="s">
         <v>68</v>
       </c>
-      <c r="C183" s="37">
+      <c r="C183" s="43">
         <v>24000</v>
       </c>
     </row>
@@ -3552,7 +3567,7 @@
       <c r="B184" t="s">
         <v>60</v>
       </c>
-      <c r="C184" s="37">
+      <c r="C184" s="43">
         <v>11000</v>
       </c>
     </row>
@@ -3563,7 +3578,7 @@
       <c r="B185" t="s">
         <v>60</v>
       </c>
-      <c r="C185" s="37">
+      <c r="C185" s="43">
         <v>10000</v>
       </c>
     </row>
@@ -3574,7 +3589,7 @@
       <c r="B186" t="s">
         <v>36</v>
       </c>
-      <c r="C186" s="37">
+      <c r="C186" s="43">
         <v>26000</v>
       </c>
     </row>
@@ -3585,7 +3600,7 @@
       <c r="B187" t="s">
         <v>68</v>
       </c>
-      <c r="C187" s="37">
+      <c r="C187" s="43">
         <v>0</v>
       </c>
     </row>
@@ -3596,7 +3611,7 @@
       <c r="B188" t="s">
         <v>60</v>
       </c>
-      <c r="C188" s="37">
+      <c r="C188" s="43">
         <v>22000</v>
       </c>
     </row>
@@ -3607,7 +3622,7 @@
       <c r="B189" t="s">
         <v>60</v>
       </c>
-      <c r="C189" s="37">
+      <c r="C189" s="43">
         <v>63000</v>
       </c>
     </row>
@@ -3618,7 +3633,7 @@
       <c r="B190" t="s">
         <v>36</v>
       </c>
-      <c r="C190" s="37">
+      <c r="C190" s="43">
         <v>63000</v>
       </c>
     </row>
@@ -3629,7 +3644,7 @@
       <c r="B191" t="s">
         <v>78</v>
       </c>
-      <c r="C191" s="37">
+      <c r="C191" s="43">
         <v>26000</v>
       </c>
     </row>
@@ -3640,7 +3655,7 @@
       <c r="B192" t="s">
         <v>70</v>
       </c>
-      <c r="C192" s="37">
+      <c r="C192" s="43">
         <v>25000</v>
       </c>
     </row>
@@ -3651,7 +3666,7 @@
       <c r="B193" t="s">
         <v>60</v>
       </c>
-      <c r="C193" s="37">
+      <c r="C193" s="43">
         <v>25000</v>
       </c>
     </row>
@@ -3662,7 +3677,7 @@
       <c r="B194" t="s">
         <v>60</v>
       </c>
-      <c r="C194" s="37">
+      <c r="C194" s="43">
         <v>46000</v>
       </c>
     </row>
@@ -3673,7 +3688,7 @@
       <c r="B195" t="s">
         <v>40</v>
       </c>
-      <c r="C195" s="37">
+      <c r="C195" s="43">
         <v>0</v>
       </c>
     </row>
@@ -3684,7 +3699,7 @@
       <c r="B196" t="s">
         <v>49</v>
       </c>
-      <c r="C196" s="37">
+      <c r="C196" s="43">
         <v>37000</v>
       </c>
     </row>
@@ -3695,7 +3710,7 @@
       <c r="B197" t="s">
         <v>60</v>
       </c>
-      <c r="C197" s="37">
+      <c r="C197" s="43">
         <v>37000</v>
       </c>
     </row>
@@ -3706,7 +3721,7 @@
       <c r="B198" t="s">
         <v>98</v>
       </c>
-      <c r="C198" s="37">
+      <c r="C198" s="43">
         <v>11000</v>
       </c>
     </row>
@@ -3717,7 +3732,7 @@
       <c r="B199" t="s">
         <v>52</v>
       </c>
-      <c r="C199" s="37">
+      <c r="C199" s="43">
         <v>46000</v>
       </c>
     </row>
@@ -3728,7 +3743,7 @@
       <c r="B200" t="s">
         <v>54</v>
       </c>
-      <c r="C200" s="37">
+      <c r="C200" s="43">
         <v>19000</v>
       </c>
     </row>
@@ -3739,7 +3754,7 @@
       <c r="B201" t="s">
         <v>73</v>
       </c>
-      <c r="C201" s="37">
+      <c r="C201" s="43">
         <v>13000</v>
       </c>
     </row>
@@ -3750,7 +3765,7 @@
       <c r="B202" t="s">
         <v>68</v>
       </c>
-      <c r="C202" s="37">
+      <c r="C202" s="43">
         <v>26000</v>
       </c>
     </row>
@@ -3761,7 +3776,7 @@
       <c r="B203" t="s">
         <v>88</v>
       </c>
-      <c r="C203" s="37">
+      <c r="C203" s="43">
         <v>26000</v>
       </c>
     </row>
@@ -3772,7 +3787,7 @@
       <c r="B204" t="s">
         <v>36</v>
       </c>
-      <c r="C204" s="37">
+      <c r="C204" s="43">
         <v>20000</v>
       </c>
     </row>
@@ -3783,7 +3798,7 @@
       <c r="B205" t="s">
         <v>40</v>
       </c>
-      <c r="C205" s="37">
+      <c r="C205" s="43">
         <v>49000</v>
       </c>
     </row>
@@ -3794,7 +3809,7 @@
       <c r="B206" t="s">
         <v>40</v>
       </c>
-      <c r="C206" s="37">
+      <c r="C206" s="43">
         <v>33000</v>
       </c>
     </row>
@@ -3805,7 +3820,7 @@
       <c r="B207" t="s">
         <v>81</v>
       </c>
-      <c r="C207" s="37">
+      <c r="C207" s="43">
         <v>68000</v>
       </c>
     </row>
@@ -3816,7 +3831,7 @@
       <c r="B208" t="s">
         <v>52</v>
       </c>
-      <c r="C208" s="37">
+      <c r="C208" s="43">
         <v>33000</v>
       </c>
     </row>
@@ -3827,7 +3842,7 @@
       <c r="B209" t="s">
         <v>68</v>
       </c>
-      <c r="C209" s="37">
+      <c r="C209" s="43">
         <v>147000</v>
       </c>
     </row>
@@ -3838,7 +3853,7 @@
       <c r="B210" t="s">
         <v>81</v>
       </c>
-      <c r="C210" s="37">
+      <c r="C210" s="43">
         <v>151000</v>
       </c>
     </row>
@@ -3849,7 +3864,7 @@
       <c r="B211" t="s">
         <v>81</v>
       </c>
-      <c r="C211" s="37">
+      <c r="C211" s="43">
         <v>197000</v>
       </c>
     </row>
@@ -3860,7 +3875,7 @@
       <c r="B212" t="s">
         <v>88</v>
       </c>
-      <c r="C212" s="37">
+      <c r="C212" s="43">
         <v>310000</v>
       </c>
     </row>
@@ -3868,10 +3883,10 @@
       <c r="A213" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B213" s="38" t="s">
+      <c r="B213" s="37" t="s">
         <v>240</v>
       </c>
-      <c r="C213" s="37">
+      <c r="C213" s="43">
         <v>271000</v>
       </c>
     </row>
@@ -3882,7 +3897,7 @@
       <c r="B214" t="s">
         <v>36</v>
       </c>
-      <c r="C214" s="37">
+      <c r="C214" s="43">
         <v>458000</v>
       </c>
     </row>
@@ -3893,7 +3908,7 @@
       <c r="B215" t="s">
         <v>36</v>
       </c>
-      <c r="C215" s="37">
+      <c r="C215" s="43">
         <v>412000</v>
       </c>
     </row>
@@ -3904,7 +3919,7 @@
       <c r="B216" t="s">
         <v>36</v>
       </c>
-      <c r="C216" s="37">
+      <c r="C216" s="43">
         <v>807000</v>
       </c>
     </row>
@@ -3915,7 +3930,7 @@
       <c r="B217" t="s">
         <v>78</v>
       </c>
-      <c r="C217" s="37">
+      <c r="C217" s="43">
         <v>4000</v>
       </c>
     </row>
@@ -3926,7 +3941,7 @@
       <c r="B218" t="s">
         <v>56</v>
       </c>
-      <c r="C218" s="37">
+      <c r="C218" s="43">
         <v>81000</v>
       </c>
     </row>
@@ -3937,7 +3952,7 @@
       <c r="B219" t="s">
         <v>94</v>
       </c>
-      <c r="C219" s="37">
+      <c r="C219" s="43">
         <v>125000</v>
       </c>
     </row>
@@ -3948,7 +3963,7 @@
       <c r="B220" t="s">
         <v>81</v>
       </c>
-      <c r="C220" s="37">
+      <c r="C220" s="43">
         <v>98000</v>
       </c>
     </row>
@@ -3959,7 +3974,7 @@
       <c r="B221" t="s">
         <v>36</v>
       </c>
-      <c r="C221" s="37">
+      <c r="C221" s="43">
         <v>140000</v>
       </c>
     </row>
@@ -3970,7 +3985,7 @@
       <c r="B222" t="s">
         <v>40</v>
       </c>
-      <c r="C222" s="37">
+      <c r="C222" s="43">
         <v>5000</v>
       </c>
     </row>
@@ -3981,7 +3996,7 @@
       <c r="B223" t="s">
         <v>94</v>
       </c>
-      <c r="C223" s="37">
+      <c r="C223" s="43">
         <v>6000</v>
       </c>
     </row>
@@ -3992,7 +4007,7 @@
       <c r="B224" t="s">
         <v>40</v>
       </c>
-      <c r="C224" s="37">
+      <c r="C224" s="43">
         <v>9000</v>
       </c>
     </row>
@@ -4003,7 +4018,7 @@
       <c r="B225" t="s">
         <v>88</v>
       </c>
-      <c r="C225" s="37">
+      <c r="C225" s="43">
         <v>8000</v>
       </c>
     </row>
@@ -4014,7 +4029,7 @@
       <c r="B226" t="s">
         <v>88</v>
       </c>
-      <c r="C226" s="37">
+      <c r="C226" s="43">
         <v>11000</v>
       </c>
     </row>
@@ -4025,7 +4040,7 @@
       <c r="B227" t="s">
         <v>94</v>
       </c>
-      <c r="C227" s="37">
+      <c r="C227" s="43">
         <v>21000</v>
       </c>
     </row>
@@ -4036,7 +4051,7 @@
       <c r="B228" t="s">
         <v>102</v>
       </c>
-      <c r="C228" s="37">
+      <c r="C228" s="43">
         <v>14000</v>
       </c>
     </row>
@@ -4047,7 +4062,7 @@
       <c r="B229" t="s">
         <v>58</v>
       </c>
-      <c r="C229" s="37">
+      <c r="C229" s="43">
         <v>23000</v>
       </c>
     </row>
@@ -4058,7 +4073,7 @@
       <c r="B230" t="s">
         <v>68</v>
       </c>
-      <c r="C230" s="37">
+      <c r="C230" s="43">
         <v>51000</v>
       </c>
     </row>
@@ -4069,7 +4084,7 @@
       <c r="B231" t="s">
         <v>68</v>
       </c>
-      <c r="C231" s="37">
+      <c r="C231" s="43">
         <v>0</v>
       </c>
     </row>
@@ -4080,7 +4095,7 @@
       <c r="B232" t="s">
         <v>54</v>
       </c>
-      <c r="C232" s="37">
+      <c r="C232" s="43">
         <v>198000</v>
       </c>
     </row>
@@ -4091,7 +4106,7 @@
       <c r="B233" t="s">
         <v>102</v>
       </c>
-      <c r="C233" s="37">
+      <c r="C233" s="43">
         <v>167000</v>
       </c>
     </row>
@@ -4102,7 +4117,7 @@
       <c r="B234" t="s">
         <v>56</v>
       </c>
-      <c r="C234" s="37">
+      <c r="C234" s="43">
         <v>95000</v>
       </c>
     </row>
@@ -4113,7 +4128,7 @@
       <c r="B235" t="s">
         <v>94</v>
       </c>
-      <c r="C235" s="37">
+      <c r="C235" s="43">
         <v>141000</v>
       </c>
     </row>
@@ -4124,7 +4139,7 @@
       <c r="B236" t="s">
         <v>58</v>
       </c>
-      <c r="C236" s="37">
+      <c r="C236" s="43">
         <v>351000</v>
       </c>
     </row>
@@ -4135,7 +4150,7 @@
       <c r="B237" t="s">
         <v>36</v>
       </c>
-      <c r="C237" s="37">
+      <c r="C237" s="43">
         <v>414000</v>
       </c>
     </row>
@@ -4146,7 +4161,7 @@
       <c r="B238" t="s">
         <v>52</v>
       </c>
-      <c r="C238" s="37">
+      <c r="C238" s="43">
         <v>61000</v>
       </c>
     </row>
@@ -4157,7 +4172,7 @@
       <c r="B239" t="s">
         <v>68</v>
       </c>
-      <c r="C239" s="37">
+      <c r="C239" s="43">
         <v>893000</v>
       </c>
     </row>
@@ -4168,7 +4183,7 @@
       <c r="B240" t="s">
         <v>68</v>
       </c>
-      <c r="C240" s="37">
+      <c r="C240" s="43">
         <v>985000</v>
       </c>
     </row>
@@ -4179,7 +4194,7 @@
       <c r="B241" t="s">
         <v>94</v>
       </c>
-      <c r="C241" s="37">
+      <c r="C241" s="43">
         <v>296000</v>
       </c>
     </row>
@@ -4190,7 +4205,7 @@
       <c r="B242" t="s">
         <v>36</v>
       </c>
-      <c r="C242" s="37">
+      <c r="C242" s="43">
         <v>685000</v>
       </c>
     </row>
@@ -4201,7 +4216,7 @@
       <c r="B243" t="s">
         <v>36</v>
       </c>
-      <c r="C243" s="37">
+      <c r="C243" s="43">
         <v>1138000</v>
       </c>
     </row>
@@ -4212,7 +4227,7 @@
       <c r="B244" t="s">
         <v>68</v>
       </c>
-      <c r="C244" s="37">
+      <c r="C244" s="43">
         <v>1334000</v>
       </c>
     </row>
@@ -4223,7 +4238,7 @@
       <c r="B245" t="s">
         <v>58</v>
       </c>
-      <c r="C245" s="37">
+      <c r="C245" s="43">
         <v>30000</v>
       </c>
     </row>
@@ -4234,7 +4249,7 @@
       <c r="B246" t="s">
         <v>56</v>
       </c>
-      <c r="C246" s="37">
+      <c r="C246" s="43">
         <v>30000</v>
       </c>
     </row>
@@ -4245,7 +4260,7 @@
       <c r="B247" t="s">
         <v>44</v>
       </c>
-      <c r="C247" s="37">
+      <c r="C247" s="43">
         <v>406000</v>
       </c>
     </row>
@@ -4256,7 +4271,7 @@
       <c r="B248" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="C248" s="37">
+      <c r="C248" s="43">
         <v>197000</v>
       </c>
     </row>
@@ -4267,7 +4282,7 @@
       <c r="B249" t="s">
         <v>68</v>
       </c>
-      <c r="C249" s="37">
+      <c r="C249" s="43">
         <v>645000</v>
       </c>
     </row>
@@ -4278,7 +4293,7 @@
       <c r="B250" t="s">
         <v>46</v>
       </c>
-      <c r="C250" s="37">
+      <c r="C250" s="43">
         <v>645000</v>
       </c>
     </row>
@@ -4289,7 +4304,7 @@
       <c r="B251" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="C251" s="37">
+      <c r="C251" s="43">
         <v>259000</v>
       </c>
     </row>
@@ -4300,7 +4315,7 @@
       <c r="B252" t="s">
         <v>38</v>
       </c>
-      <c r="C252" s="37">
+      <c r="C252" s="43">
         <v>646000</v>
       </c>
     </row>
@@ -4311,7 +4326,7 @@
       <c r="B253" t="s">
         <v>78</v>
       </c>
-      <c r="C253" s="37">
+      <c r="C253" s="43">
         <v>259000</v>
       </c>
     </row>
@@ -4322,7 +4337,7 @@
       <c r="B254" t="s">
         <v>98</v>
       </c>
-      <c r="C254" s="37">
+      <c r="C254" s="43">
         <v>645000</v>
       </c>
     </row>
@@ -4333,7 +4348,7 @@
       <c r="B255" t="s">
         <v>68</v>
       </c>
-      <c r="C255" s="37">
+      <c r="C255" s="43">
         <v>879000</v>
       </c>
     </row>
@@ -4344,7 +4359,7 @@
       <c r="B256" t="s">
         <v>42</v>
       </c>
-      <c r="C256" s="37">
+      <c r="C256" s="43">
         <v>259000</v>
       </c>
     </row>
@@ -4355,7 +4370,7 @@
       <c r="B257" t="s">
         <v>42</v>
       </c>
-      <c r="C257" s="37">
+      <c r="C257" s="43">
         <v>274000</v>
       </c>
     </row>
@@ -4366,7 +4381,7 @@
       <c r="B258" t="s">
         <v>52</v>
       </c>
-      <c r="C258" s="37">
+      <c r="C258" s="43">
         <v>975000</v>
       </c>
     </row>
@@ -4377,7 +4392,7 @@
       <c r="B259" t="s">
         <v>36</v>
       </c>
-      <c r="C259" s="37">
+      <c r="C259" s="43">
         <v>480000</v>
       </c>
     </row>
@@ -4388,7 +4403,7 @@
       <c r="B260" t="s">
         <v>56</v>
       </c>
-      <c r="C260" s="37">
+      <c r="C260" s="43">
         <v>1187000</v>
       </c>
     </row>
@@ -4399,7 +4414,7 @@
       <c r="B261" t="s">
         <v>40</v>
       </c>
-      <c r="C261" s="37">
+      <c r="C261" s="43">
         <v>832000</v>
       </c>
     </row>
@@ -4410,7 +4425,7 @@
       <c r="B262" t="s">
         <v>68</v>
       </c>
-      <c r="C262" s="37">
+      <c r="C262" s="43">
         <v>227000</v>
       </c>
     </row>
@@ -4421,7 +4436,7 @@
       <c r="B263" t="s">
         <v>60</v>
       </c>
-      <c r="C263" s="37">
+      <c r="C263" s="43">
         <v>98000</v>
       </c>
     </row>
@@ -4432,7 +4447,7 @@
       <c r="B264" t="s">
         <v>60</v>
       </c>
-      <c r="C264" s="37">
+      <c r="C264" s="43">
         <v>1190000</v>
       </c>
     </row>
@@ -4443,7 +4458,7 @@
       <c r="B265" t="s">
         <v>36</v>
       </c>
-      <c r="C265" s="37">
+      <c r="C265" s="43">
         <v>300000</v>
       </c>
     </row>
@@ -4454,7 +4469,7 @@
       <c r="B266" t="s">
         <v>68</v>
       </c>
-      <c r="C266" s="37">
+      <c r="C266" s="43">
         <v>2407000</v>
       </c>
     </row>
@@ -4465,7 +4480,7 @@
       <c r="B267" t="s">
         <v>60</v>
       </c>
-      <c r="C267" s="37">
+      <c r="C267" s="43">
         <v>1021000</v>
       </c>
     </row>
@@ -4476,7 +4491,7 @@
       <c r="B268" t="s">
         <v>60</v>
       </c>
-      <c r="C268" s="37">
+      <c r="C268" s="43">
         <v>646000</v>
       </c>
     </row>
@@ -4487,7 +4502,7 @@
       <c r="B269" t="s">
         <v>36</v>
       </c>
-      <c r="C269" s="37">
+      <c r="C269" s="43">
         <v>259000</v>
       </c>
     </row>
@@ -4498,7 +4513,7 @@
       <c r="B270" t="s">
         <v>78</v>
       </c>
-      <c r="C270" s="37">
+      <c r="C270" s="43">
         <v>193000</v>
       </c>
     </row>
@@ -4509,7 +4524,7 @@
       <c r="B271" t="s">
         <v>70</v>
       </c>
-      <c r="C271" s="37">
+      <c r="C271" s="43">
         <v>96000</v>
       </c>
     </row>
@@ -4520,7 +4535,7 @@
       <c r="B272" t="s">
         <v>60</v>
       </c>
-      <c r="C272" s="37">
+      <c r="C272" s="43">
         <v>594000</v>
       </c>
     </row>
@@ -4531,7 +4546,7 @@
       <c r="B273" t="s">
         <v>60</v>
       </c>
-      <c r="C273" s="37">
+      <c r="C273" s="43">
         <v>282000</v>
       </c>
     </row>
@@ -4542,7 +4557,7 @@
       <c r="B274" t="s">
         <v>40</v>
       </c>
-      <c r="C274" s="37">
+      <c r="C274" s="43">
         <v>1814000</v>
       </c>
     </row>
@@ -4553,7 +4568,7 @@
       <c r="B275" t="s">
         <v>49</v>
       </c>
-      <c r="C275" s="37">
+      <c r="C275" s="43">
         <v>193000</v>
       </c>
     </row>
@@ -4564,7 +4579,7 @@
       <c r="B276" t="s">
         <v>60</v>
       </c>
-      <c r="C276" s="37">
+      <c r="C276" s="43">
         <v>654000</v>
       </c>
     </row>
@@ -4575,7 +4590,7 @@
       <c r="B277" t="s">
         <v>98</v>
       </c>
-      <c r="C277" s="37">
+      <c r="C277" s="43">
         <v>729000</v>
       </c>
     </row>
@@ -4586,7 +4601,7 @@
       <c r="B278" t="s">
         <v>52</v>
       </c>
-      <c r="C278" s="37">
+      <c r="C278" s="43">
         <v>632000</v>
       </c>
     </row>
@@ -4597,7 +4612,7 @@
       <c r="B279" t="s">
         <v>54</v>
       </c>
-      <c r="C279" s="37">
+      <c r="C279" s="43">
         <v>240000</v>
       </c>
     </row>
@@ -4608,7 +4623,7 @@
       <c r="B280" t="s">
         <v>73</v>
       </c>
-      <c r="C280" s="37">
+      <c r="C280" s="43">
         <v>955000</v>
       </c>
     </row>
@@ -4619,7 +4634,7 @@
       <c r="B281" t="s">
         <v>68</v>
       </c>
-      <c r="C281" s="37">
+      <c r="C281" s="43">
         <v>1126000</v>
       </c>
     </row>
@@ -4630,7 +4645,7 @@
       <c r="B282" t="s">
         <v>88</v>
       </c>
-      <c r="C282" s="37">
+      <c r="C282" s="43">
         <v>0</v>
       </c>
     </row>
@@ -4641,7 +4656,7 @@
       <c r="B283" t="s">
         <v>36</v>
       </c>
-      <c r="C283" s="37">
+      <c r="C283" s="43">
         <v>297000</v>
       </c>
     </row>
@@ -4652,7 +4667,7 @@
       <c r="B284" t="s">
         <v>40</v>
       </c>
-      <c r="C284" s="37">
+      <c r="C284" s="43">
         <v>646000</v>
       </c>
     </row>
@@ -4663,7 +4678,7 @@
       <c r="B285" t="s">
         <v>40</v>
       </c>
-      <c r="C285" s="37">
+      <c r="C285" s="43">
         <v>714000</v>
       </c>
     </row>
@@ -4674,7 +4689,7 @@
       <c r="B286" t="s">
         <v>81</v>
       </c>
-      <c r="C286" s="37">
+      <c r="C286" s="43">
         <v>807000</v>
       </c>
     </row>
@@ -4685,7 +4700,7 @@
       <c r="B287" t="s">
         <v>52</v>
       </c>
-      <c r="C287" s="37">
+      <c r="C287" s="43">
         <v>591000</v>
       </c>
     </row>
@@ -4696,7 +4711,7 @@
       <c r="B288" t="s">
         <v>68</v>
       </c>
-      <c r="C288" s="37">
+      <c r="C288" s="43">
         <v>918000</v>
       </c>
     </row>
@@ -4707,7 +4722,7 @@
       <c r="B289" t="s">
         <v>81</v>
       </c>
-      <c r="C289" s="37">
+      <c r="C289" s="43">
         <v>1265000</v>
       </c>
     </row>
@@ -4718,7 +4733,7 @@
       <c r="B290" t="s">
         <v>81</v>
       </c>
-      <c r="C290" s="37">
+      <c r="C290" s="43">
         <v>256000</v>
       </c>
     </row>
@@ -4729,7 +4744,7 @@
       <c r="B291" t="s">
         <v>88</v>
       </c>
-      <c r="C291" s="37">
+      <c r="C291" s="43">
         <v>371000</v>
       </c>
     </row>
@@ -4737,10 +4752,10 @@
       <c r="A292" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B292" s="38" t="s">
+      <c r="B292" s="37" t="s">
         <v>240</v>
       </c>
-      <c r="C292" s="37">
+      <c r="C292" s="43">
         <v>457000</v>
       </c>
     </row>
@@ -4751,7 +4766,7 @@
       <c r="B293" t="s">
         <v>36</v>
       </c>
-      <c r="C293" s="37">
+      <c r="C293" s="43">
         <v>642000</v>
       </c>
     </row>
@@ -4762,7 +4777,7 @@
       <c r="B294" t="s">
         <v>36</v>
       </c>
-      <c r="C294" s="37">
+      <c r="C294" s="43">
         <v>1571000</v>
       </c>
     </row>
@@ -4773,7 +4788,7 @@
       <c r="B295" t="s">
         <v>36</v>
       </c>
-      <c r="C295" s="37">
+      <c r="C295" s="43">
         <v>756000</v>
       </c>
     </row>
@@ -4784,7 +4799,7 @@
       <c r="B296" t="s">
         <v>78</v>
       </c>
-      <c r="C296" s="37">
+      <c r="C296" s="43">
         <v>1571000</v>
       </c>
     </row>
@@ -4795,7 +4810,7 @@
       <c r="B297" t="s">
         <v>56</v>
       </c>
-      <c r="C297" s="37">
+      <c r="C297" s="43">
         <v>2716000</v>
       </c>
     </row>
@@ -4806,7 +4821,7 @@
       <c r="B298" t="s">
         <v>94</v>
       </c>
-      <c r="C298" s="37">
+      <c r="C298" s="43">
         <v>640000</v>
       </c>
     </row>
@@ -4817,7 +4832,7 @@
       <c r="B299" t="s">
         <v>81</v>
       </c>
-      <c r="C299" s="37">
+      <c r="C299" s="43">
         <v>255000</v>
       </c>
     </row>
@@ -4828,7 +4843,7 @@
       <c r="B300" t="s">
         <v>36</v>
       </c>
-      <c r="C300" s="37">
+      <c r="C300" s="43">
         <v>413000</v>
       </c>
     </row>
@@ -4839,7 +4854,7 @@
       <c r="B301" t="s">
         <v>40</v>
       </c>
-      <c r="C301" s="37">
+      <c r="C301" s="43">
         <v>361000</v>
       </c>
     </row>
@@ -4850,7 +4865,7 @@
       <c r="B302" t="s">
         <v>94</v>
       </c>
-      <c r="C302" s="37">
+      <c r="C302" s="43">
         <v>544000</v>
       </c>
     </row>
@@ -4861,7 +4876,7 @@
       <c r="B303" t="s">
         <v>40</v>
       </c>
-      <c r="C303" s="37">
+      <c r="C303" s="43">
         <v>678000</v>
       </c>
     </row>
@@ -4872,7 +4887,7 @@
       <c r="B304" t="s">
         <v>88</v>
       </c>
-      <c r="C304" s="37">
+      <c r="C304" s="43">
         <v>1054000</v>
       </c>
     </row>
@@ -4883,7 +4898,7 @@
       <c r="B305" t="s">
         <v>88</v>
       </c>
-      <c r="C305" s="37">
+      <c r="C305" s="43">
         <v>482000</v>
       </c>
     </row>
@@ -4894,7 +4909,7 @@
       <c r="B306" t="s">
         <v>94</v>
       </c>
-      <c r="C306" s="37">
+      <c r="C306" s="43">
         <v>722000</v>
       </c>
     </row>
@@ -4905,7 +4920,7 @@
       <c r="B307" t="s">
         <v>102</v>
       </c>
-      <c r="C307" s="37">
+      <c r="C307" s="43">
         <v>269000</v>
       </c>
     </row>
@@ -4916,7 +4931,7 @@
       <c r="B308" t="s">
         <v>58</v>
       </c>
-      <c r="C308" s="37">
+      <c r="C308" s="43">
         <v>371000</v>
       </c>
     </row>
@@ -4927,7 +4942,7 @@
       <c r="B309" t="s">
         <v>68</v>
       </c>
-      <c r="C309" s="37">
+      <c r="C309" s="43">
         <v>462000</v>
       </c>
     </row>
@@ -4938,7 +4953,7 @@
       <c r="B310" t="s">
         <v>68</v>
       </c>
-      <c r="C310" s="37">
+      <c r="C310" s="43">
         <v>541000</v>
       </c>
     </row>
@@ -4949,7 +4964,7 @@
       <c r="B311" t="s">
         <v>54</v>
       </c>
-      <c r="C311" s="37">
+      <c r="C311" s="43">
         <v>648000</v>
       </c>
     </row>
@@ -4960,7 +4975,7 @@
       <c r="B312" t="s">
         <v>102</v>
       </c>
-      <c r="C312" s="37">
+      <c r="C312" s="43">
         <v>644000</v>
       </c>
     </row>
@@ -4971,7 +4986,7 @@
       <c r="B313" t="s">
         <v>56</v>
       </c>
-      <c r="C313" s="37">
+      <c r="C313" s="43">
         <v>902000</v>
       </c>
     </row>
@@ -4982,7 +4997,7 @@
       <c r="B314" t="s">
         <v>94</v>
       </c>
-      <c r="C314" s="37">
+      <c r="C314" s="43">
         <v>722000</v>
       </c>
     </row>
@@ -4993,7 +5008,7 @@
       <c r="B315" t="s">
         <v>58</v>
       </c>
-      <c r="C315" s="37">
+      <c r="C315" s="43">
         <v>1457000</v>
       </c>
     </row>
@@ -5004,7 +5019,7 @@
       <c r="B316" t="s">
         <v>36</v>
       </c>
-      <c r="C316" s="37">
+      <c r="C316" s="43">
         <v>1786000</v>
       </c>
     </row>
@@ -5015,7 +5030,7 @@
       <c r="B317" t="s">
         <v>52</v>
       </c>
-      <c r="C317" s="37">
+      <c r="C317" s="43">
         <v>0</v>
       </c>
     </row>
@@ -5026,7 +5041,7 @@
       <c r="B318" t="s">
         <v>68</v>
       </c>
-      <c r="C318" s="37">
+      <c r="C318" s="43">
         <v>85000</v>
       </c>
     </row>
@@ -5037,7 +5052,7 @@
       <c r="B319" t="s">
         <v>68</v>
       </c>
-      <c r="C319" s="37">
+      <c r="C319" s="43">
         <v>84000</v>
       </c>
     </row>
@@ -5048,7 +5063,7 @@
       <c r="B320" t="s">
         <v>94</v>
       </c>
-      <c r="C320" s="37">
+      <c r="C320" s="43">
         <v>115000</v>
       </c>
     </row>
@@ -5059,7 +5074,7 @@
       <c r="B321" t="s">
         <v>36</v>
       </c>
-      <c r="C321" s="37">
+      <c r="C321" s="43">
         <v>152000</v>
       </c>
     </row>
@@ -5070,7 +5085,7 @@
       <c r="B322" t="s">
         <v>36</v>
       </c>
-      <c r="C322" s="37">
+      <c r="C322" s="43">
         <v>82000</v>
       </c>
     </row>
@@ -5081,7 +5096,7 @@
       <c r="B323" t="s">
         <v>68</v>
       </c>
-      <c r="C323" s="37">
+      <c r="C323" s="43">
         <v>84000</v>
       </c>
     </row>
@@ -5092,7 +5107,7 @@
       <c r="B324" t="s">
         <v>58</v>
       </c>
-      <c r="C324" s="37">
+      <c r="C324" s="43">
         <v>115000</v>
       </c>
     </row>
@@ -5103,7 +5118,7 @@
       <c r="B325" t="s">
         <v>56</v>
       </c>
-      <c r="C325" s="37">
+      <c r="C325" s="43">
         <v>153000</v>
       </c>
     </row>
@@ -5114,7 +5129,7 @@
       <c r="B326" t="s">
         <v>44</v>
       </c>
-      <c r="C326" s="37">
+      <c r="C326" s="43">
         <v>80000</v>
       </c>
     </row>
@@ -5125,7 +5140,7 @@
       <c r="B327" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="C327" s="37">
+      <c r="C327" s="43">
         <v>102000</v>
       </c>
     </row>
@@ -5136,7 +5151,7 @@
       <c r="B328" t="s">
         <v>68</v>
       </c>
-      <c r="C328" s="37">
+      <c r="C328" s="43">
         <v>0</v>
       </c>
     </row>
@@ -5147,7 +5162,7 @@
       <c r="B329" t="s">
         <v>46</v>
       </c>
-      <c r="C329" s="37">
+      <c r="C329" s="43">
         <v>198000</v>
       </c>
     </row>
@@ -5158,7 +5173,7 @@
       <c r="B330" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="C330" s="37">
+      <c r="C330" s="43">
         <v>233000</v>
       </c>
     </row>
@@ -5169,7 +5184,7 @@
       <c r="B331" t="s">
         <v>38</v>
       </c>
-      <c r="C331" s="37">
+      <c r="C331" s="43">
         <v>279000</v>
       </c>
     </row>
@@ -5180,7 +5195,7 @@
       <c r="B332" t="s">
         <v>78</v>
       </c>
-      <c r="C332" s="37">
+      <c r="C332" s="43">
         <v>298000</v>
       </c>
     </row>
@@ -5191,7 +5206,7 @@
       <c r="B333" t="s">
         <v>98</v>
       </c>
-      <c r="C333" s="37">
+      <c r="C333" s="43">
         <v>478000</v>
       </c>
     </row>
@@ -5202,7 +5217,7 @@
       <c r="B334" t="s">
         <v>68</v>
       </c>
-      <c r="C334" s="37">
+      <c r="C334" s="43">
         <v>626000</v>
       </c>
     </row>
@@ -5213,7 +5228,7 @@
       <c r="B335" t="s">
         <v>42</v>
       </c>
-      <c r="C335" s="37">
+      <c r="C335" s="43">
         <v>757000</v>
       </c>
     </row>
@@ -5224,7 +5239,7 @@
       <c r="B336" t="s">
         <v>42</v>
       </c>
-      <c r="C336" s="37">
+      <c r="C336" s="43">
         <v>1128000</v>
       </c>
     </row>
@@ -5235,7 +5250,7 @@
       <c r="B337" t="s">
         <v>52</v>
       </c>
-      <c r="C337" s="37">
+      <c r="C337" s="43">
         <v>1527000</v>
       </c>
     </row>
@@ -5246,7 +5261,7 @@
       <c r="B338" t="s">
         <v>36</v>
       </c>
-      <c r="C338" s="37">
+      <c r="C338" s="43">
         <v>4134000</v>
       </c>
     </row>
@@ -5257,7 +5272,7 @@
       <c r="B339" t="s">
         <v>56</v>
       </c>
-      <c r="C339" s="37">
+      <c r="C339" s="43">
         <v>6850000</v>
       </c>
     </row>
@@ -5268,8 +5283,26 @@
       <c r="B340" t="s">
         <v>40</v>
       </c>
-      <c r="C340" s="37">
+      <c r="C340" s="43">
         <v>11712000</v>
+      </c>
+    </row>
+    <row r="342" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C342" s="9">
+        <f>SUM(C5:C340)</f>
+        <v>171416000</v>
+      </c>
+      <c r="D342" s="7" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="343" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C343" s="9">
+        <f>AVERAGE(C5:C340)</f>
+        <v>510166.66666666669</v>
+      </c>
+      <c r="D343" s="7" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="345" spans="1:6" x14ac:dyDescent="0.2">
@@ -5282,9 +5315,47 @@
     <mergeCell ref="A3:C3"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
+  <conditionalFormatting sqref="B5:B340">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"Ufficio"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:C340">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFB628"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{DBC5AE29-9CB2-42DE-8DBA-32C72F24863B}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{DBC5AE29-9CB2-42DE-8DBA-32C72F24863B}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFFB628"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>C5:C340</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5292,8 +5363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H80"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6770,7 +6841,7 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6825,14 +6896,14 @@
         <f>IF(AND(A2="gennaio",C2="casa",E2&gt;10),"Trovato","")</f>
         <v/>
       </c>
-      <c r="G2" s="42" t="s">
+      <c r="G2" s="41" t="s">
         <v>225</v>
       </c>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
@@ -6854,12 +6925,12 @@
         <f t="shared" ref="F3:F24" si="0">IF(AND(A3="gennaio",C3="casa",E3&gt;10),"Trovato","")</f>
         <v>Trovato</v>
       </c>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
@@ -6881,12 +6952,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
-      <c r="L4" s="43"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
@@ -6908,12 +6979,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43"/>
-      <c r="L5" s="43"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="42"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
@@ -6935,12 +7006,12 @@
         <f t="shared" si="0"/>
         <v>Trovato</v>
       </c>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
-      <c r="L6" s="43"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="42"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
@@ -6962,12 +7033,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="43"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="42"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
@@ -6989,12 +7060,12 @@
         <f t="shared" si="0"/>
         <v>Trovato</v>
       </c>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="43"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">

</xml_diff>